<commit_message>
+ shadow-aligment_train.json as unsafe
</commit_message>
<xml_diff>
--- a/merging_results.xlsx
+++ b/merging_results.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\笔记\all_notes\data\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_ssh\model_merging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0423B6BC-0AD7-4E99-B9C4-089248E14374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A8A000-E2E9-486A-BB50-7C241348D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="泛化性能测试" sheetId="1" r:id="rId1"/>
+    <sheet name="安全性-CATQA" sheetId="2" r:id="rId2"/>
+    <sheet name="安全性-BeaverTails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,7 +98,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>+SFT</t>
+    <t>+SFT +100 unsafe data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Llama-2-chat-7B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">+SFT +100 unsafe data  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v.s.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Safe Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mask realigned</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +153,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -165,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,10 +227,28 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,14 +533,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="12" max="12" width="13.44140625" customWidth="1"/>
   </cols>
@@ -495,23 +552,21 @@
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -581,16 +636,30 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="C4">
+        <v>60.8</v>
+      </c>
+      <c r="E4">
+        <v>87</v>
+      </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="C5">
+        <v>64.2</v>
+      </c>
+      <c r="E5">
+        <v>89</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -604,4 +673,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BB2219-160D-4F49-A573-B2EED4E6EDAC}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>49.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE49E546-3C64-43C5-9161-5DD84088B964}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ update safety evaluation
</commit_message>
<xml_diff>
--- a/merging_results.xlsx
+++ b/merging_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_ssh\model_merging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130908DA-49E2-45D9-8A85-26391FA86830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D958705E-1D9E-4109-878C-71BF3F45967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="670" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="泛化性能测试" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -210,11 +211,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -236,35 +234,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -561,122 +566,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="11" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="7" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>60.8</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="16">
+        <v>61.6</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16">
         <v>87</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>64.2</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="16">
+        <v>64</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
         <v>89</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -695,7 +716,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -708,96 +729,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
+        <v>44.04</v>
+      </c>
+      <c r="G3" s="1">
         <v>49.09</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -818,7 +842,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -829,96 +853,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
+        <v>-0.72</v>
+      </c>
+      <c r="G3" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -938,7 +965,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -950,97 +977,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
+        <v>26.8</v>
+      </c>
+      <c r="G3" s="1">
         <v>41.75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1072,97 +1102,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
         <v>9.5500000000000007</v>
       </c>
+      <c r="G3" s="1">
+        <v>9.5500000000000007</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1181,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CAF58B-48A0-4F9B-8783-9A2E0FD3237B}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1194,91 +1227,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
+        <v>16.16</v>
+      </c>
+      <c r="G3" s="1">
         <v>36.869999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1292,5 +1328,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ update realign dpo
</commit_message>
<xml_diff>
--- a/merging_results.xlsx
+++ b/merging_results.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_ssh\model_merging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E3FD0E-B7B3-4BD6-91EC-8AEA300389A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53D6778-DD66-454C-AF72-D559BC0668AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="670" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="泛化性能测试" sheetId="1" r:id="rId1"/>
-    <sheet name="CATQA" sheetId="2" r:id="rId2"/>
-    <sheet name="BeaverTails" sheetId="3" r:id="rId3"/>
-    <sheet name="harmfulqa" sheetId="5" r:id="rId4"/>
-    <sheet name="shadow-alignment" sheetId="4" r:id="rId5"/>
-    <sheet name="dangerous" sheetId="6" r:id="rId6"/>
+    <sheet name="pretrain" sheetId="8" r:id="rId1"/>
+    <sheet name="泛化性能测试" sheetId="1" r:id="rId2"/>
+    <sheet name="CATQA" sheetId="2" r:id="rId3"/>
+    <sheet name="BeaverTails" sheetId="3" r:id="rId4"/>
+    <sheet name="harmfulqa" sheetId="5" r:id="rId5"/>
+    <sheet name="shadow-alignment" sheetId="4" r:id="rId6"/>
+    <sheet name="dangerous" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>+SFT +100 unsafe data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Llama-2-chat-7B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,6 +119,116 @@
   </si>
   <si>
     <t>Mask realigned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CATQA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">pku_seferlhf_pretrain_dpo_50k.json </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">pku_seferlhf_pretrain_sft_50k.json </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BeaverTails</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>harmfulqa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pku_seferlhf_pretrain_dpo_50k.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pku_seferlhf_pretrain_sft_50k.json  + pku_seferlhf_pretrain_dpo_50k.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shadow-alignment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dangerous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>best_safe_wizardlm-7b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+SFT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WizardLM-7B-Uncensored</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>best_safe_wizardlm-7b +sft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>down task Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>WizardLM-7B-Uncensored</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best_safe_wizardlm-7b</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>best_safe_wizardlm-7b +sft + unsafe 100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -133,7 +240,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +291,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -211,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,15 +338,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,6 +372,19 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -269,6 +395,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,17 +697,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B99E9F-994B-4B4D-86C2-34C99AB06792}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.77734375" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
+        <v>61.47</v>
+      </c>
+      <c r="E2" s="1">
+        <v>27.34</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44.04</v>
+      </c>
+      <c r="E6" s="1">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="27">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="E7" s="27">
+        <v>33.81</v>
+      </c>
+      <c r="F7" s="27">
+        <v>63.92</v>
+      </c>
+      <c r="G7" s="27">
+        <v>20.71</v>
+      </c>
+      <c r="H7" s="27">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="1" max="2" width="30.21875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="12" max="12" width="13.44140625" customWidth="1"/>
   </cols>
@@ -569,135 +863,133 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="19" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="16">
-        <v>61.6</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16">
+      <c r="A4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="15">
+        <v>53.8</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="15">
         <v>87</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="16">
-        <v>64</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16">
-        <v>89</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15">
+        <v>90</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -711,125 +1003,126 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BB2219-160D-4F49-A573-B2EED4E6EDAC}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44.04</v>
-      </c>
+      <c r="C3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="1"/>
       <c r="G3" s="1">
-        <v>49.09</v>
+        <v>37.61</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -837,12 +1130,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE49E546-3C64-43C5-9161-5DD84088B964}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -856,96 +1149,94 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14">
-        <v>-0.72</v>
-      </c>
-      <c r="G3" s="14">
-        <v>15</v>
+      <c r="E3" s="11"/>
+      <c r="G3" s="11">
+        <v>31.16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -960,12 +1251,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A036AD0-7582-4D92-A231-DE51ED0E95AD}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -980,97 +1271,95 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14">
-        <v>26.8</v>
-      </c>
+      <c r="E3" s="11"/>
       <c r="G3" s="1">
-        <v>38.14</v>
+        <v>29.03</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1085,12 +1374,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1D2C4E-0DC3-4E93-80C7-89BFF36994DD}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1105,97 +1394,95 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14">
-        <v>9.5500000000000007</v>
-      </c>
+      <c r="E3" s="11"/>
       <c r="G3" s="1">
-        <v>9.5500000000000007</v>
+        <v>7.61</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1210,12 +1497,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CAF58B-48A0-4F9B-8783-9A2E0FD3237B}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1231,92 +1518,90 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14">
-        <v>16.16</v>
-      </c>
+      <c r="E3" s="11"/>
       <c r="G3" s="1">
-        <v>36.869999999999997</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task vector fuse by "weight averaging"
</commit_message>
<xml_diff>
--- a/merging_results.xlsx
+++ b/merging_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_ssh\model_merging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BEEF1C-0A2A-43CA-87B5-0249CC1CA1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F41B70C-0743-4CB4-8C08-34098A6DCD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-1116" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pretrain" sheetId="8" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="shadow-alignment" sheetId="4" r:id="rId6"/>
     <sheet name="dangerousqa" sheetId="6" r:id="rId7"/>
     <sheet name="multi task" sheetId="9" r:id="rId8"/>
+    <sheet name="helpfulness" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -338,6 +339,10 @@
   </si>
   <si>
     <t>TinyLlama-1.1B --&gt;best_safe tintyllama-1.1b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESTA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,9 +572,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -577,9 +579,15 @@
     <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,6 +607,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -884,7 +904,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -924,7 +944,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -944,7 +964,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -959,15 +979,15 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="45"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="45"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -982,7 +1002,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="23" t="s">
         <v>26</v>
       </c>
@@ -1099,7 +1119,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1116,21 +1136,21 @@
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1200,7 +1220,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -1239,7 +1259,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="22" t="s">
         <v>31</v>
       </c>
@@ -1260,7 +1280,7 @@
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="14">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="J5" s="14">
         <v>39.9</v>
@@ -1276,7 +1296,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="26" t="s">
         <v>36</v>
       </c>
@@ -1295,9 +1315,24 @@
       <c r="G6" s="35">
         <v>12.2</v>
       </c>
+      <c r="I6" s="27">
+        <v>59.6</v>
+      </c>
+      <c r="J6" s="53">
+        <v>40.44</v>
+      </c>
+      <c r="K6" s="53">
+        <v>80</v>
+      </c>
+      <c r="L6" s="53">
+        <v>11.6</v>
+      </c>
+      <c r="M6" s="53">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="26" t="s">
         <v>41</v>
       </c>
@@ -1315,16 +1350,93 @@
       </c>
       <c r="G7" s="35">
         <v>10.5</v>
+      </c>
+      <c r="I7" s="53">
+        <v>60.8</v>
+      </c>
+      <c r="J7" s="53">
+        <v>40.4</v>
+      </c>
+      <c r="K7" s="53">
+        <v>80</v>
+      </c>
+      <c r="L7" s="53">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M7" s="53">
+        <v>15.2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>45</v>
       </c>
+      <c r="C8" s="27">
+        <v>60.2</v>
+      </c>
+      <c r="D8" s="27">
+        <v>40</v>
+      </c>
+      <c r="E8" s="27">
+        <v>91</v>
+      </c>
+      <c r="F8" s="27">
+        <v>10</v>
+      </c>
+      <c r="G8" s="27">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27">
+        <v>60.4</v>
+      </c>
+      <c r="J8" s="27">
+        <v>40.5</v>
+      </c>
+      <c r="K8" s="53">
+        <v>79</v>
+      </c>
+      <c r="L8" s="27">
+        <v>12.1</v>
+      </c>
+      <c r="M8" s="53">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>46</v>
+      </c>
+      <c r="C9" s="27">
+        <v>59.2</v>
+      </c>
+      <c r="D9" s="27">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E9" s="27">
+        <v>90</v>
+      </c>
+      <c r="F9" s="27">
+        <v>12.8</v>
+      </c>
+      <c r="G9" s="27">
+        <v>14.6</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27">
+        <v>57.2</v>
+      </c>
+      <c r="J9" s="27">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="K9" s="27">
+        <v>80</v>
+      </c>
+      <c r="L9" s="27">
+        <v>11.6</v>
+      </c>
+      <c r="M9" s="27">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1456,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1366,21 +1478,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="24"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1420,10 +1532,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1446,7 +1558,7 @@
         <v>37.96</v>
       </c>
       <c r="K3" s="35">
-        <v>26.61</v>
+        <v>22.94</v>
       </c>
       <c r="L3" s="37">
         <v>16.510000000000002</v>
@@ -1455,15 +1567,15 @@
         <v>32.11</v>
       </c>
       <c r="N3" s="37">
-        <v>32.11</v>
+        <v>11.11</v>
       </c>
       <c r="O3" s="37">
         <v>18.690000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -1483,17 +1595,25 @@
       <c r="I4" s="35">
         <v>60.55</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="K4" s="10">
+        <v>58.18</v>
+      </c>
+      <c r="L4" s="10">
+        <v>52.78</v>
+      </c>
       <c r="M4" s="10">
         <v>53.7</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="N4" s="10">
+        <v>17.43</v>
+      </c>
+      <c r="O4" s="10">
+        <v>50.46</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="26" t="s">
         <v>48</v>
       </c>
@@ -1512,17 +1632,103 @@
       <c r="I5" s="35">
         <v>58.72</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
+      <c r="K5" s="10">
+        <v>60.91</v>
+      </c>
+      <c r="L5" s="10">
+        <v>55.05</v>
+      </c>
+      <c r="M5" s="10">
+        <v>41.28</v>
+      </c>
+      <c r="N5" s="10">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="O5" s="10">
+        <v>41.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10">
+        <v>43.52</v>
+      </c>
+      <c r="F6" s="10">
+        <v>32</v>
+      </c>
+      <c r="G6" s="10">
+        <v>50.93</v>
+      </c>
+      <c r="H6" s="10">
+        <v>53.54</v>
+      </c>
+      <c r="I6" s="10">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="K6" s="10">
+        <v>17.43</v>
+      </c>
+      <c r="L6" s="10">
+        <v>26.85</v>
+      </c>
+      <c r="M6" s="10">
+        <v>44.04</v>
+      </c>
+      <c r="N6" s="10">
+        <v>15.6</v>
+      </c>
+      <c r="O6" s="10">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="10">
+        <v>59.22</v>
+      </c>
+      <c r="F7" s="10">
+        <v>49.51</v>
+      </c>
+      <c r="G7" s="10">
+        <v>73.53</v>
+      </c>
+      <c r="H7" s="10">
+        <v>41.35</v>
+      </c>
+      <c r="I7" s="10">
+        <v>37.11</v>
+      </c>
+      <c r="K7" s="10">
+        <v>41.82</v>
+      </c>
+      <c r="L7" s="10">
+        <v>41.82</v>
+      </c>
+      <c r="M7" s="10">
+        <v>32.409999999999997</v>
+      </c>
+      <c r="N7" s="10">
+        <v>42.2</v>
+      </c>
+      <c r="O7" s="10">
+        <v>37.270000000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
+      <c r="N9" s="42"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G12" s="1"/>
+      <c r="M12" s="42"/>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
@@ -1531,8 +1737,8 @@
   <mergeCells count="4">
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A3:A7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1545,7 +1751,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1565,21 +1771,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="16"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1619,10 +1825,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1645,22 +1851,24 @@
         <v>-19.57</v>
       </c>
       <c r="K3" s="10">
-        <v>41.73</v>
-      </c>
-      <c r="L3" s="39">
+        <v>35.25</v>
+      </c>
+      <c r="L3" s="51">
         <v>33.94</v>
       </c>
       <c r="M3" s="10">
         <v>36.229999999999997</v>
       </c>
-      <c r="N3" s="39"/>
+      <c r="N3" s="10">
+        <v>16.43</v>
+      </c>
       <c r="O3" s="10">
         <v>25.18</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="26" t="s">
         <v>16</v>
       </c>
@@ -1680,17 +1888,25 @@
       <c r="I4" s="35">
         <v>5.1100000000000003</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="K4" s="10">
+        <v>55.07</v>
+      </c>
+      <c r="L4" s="51">
+        <v>41.01</v>
+      </c>
       <c r="M4" s="10">
         <v>46.04</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="N4" s="10">
+        <v>19.57</v>
+      </c>
+      <c r="O4" s="10">
+        <v>31.65</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="26" t="s">
         <v>48</v>
       </c>
@@ -1709,14 +1925,95 @@
       <c r="I5" s="35">
         <v>11.51</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
+      <c r="K5" s="10">
+        <v>54.29</v>
+      </c>
+      <c r="L5" s="10">
+        <v>50.72</v>
+      </c>
+      <c r="M5" s="10">
+        <v>48.2</v>
+      </c>
+      <c r="N5" s="10">
+        <v>34.78</v>
+      </c>
+      <c r="O5" s="10">
+        <v>34.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="42">
+        <v>26.09</v>
+      </c>
+      <c r="F6" s="42">
+        <v>15.27</v>
+      </c>
+      <c r="G6" s="42">
+        <v>25.36</v>
+      </c>
+      <c r="H6" s="42">
+        <v>2.29</v>
+      </c>
+      <c r="I6" s="42">
+        <v>-20.9</v>
+      </c>
+      <c r="K6" s="10">
+        <v>38.57</v>
+      </c>
+      <c r="L6" s="42">
+        <v>39.130000000000003</v>
+      </c>
+      <c r="M6" s="10">
+        <v>36.69</v>
+      </c>
+      <c r="N6" s="10">
+        <v>18.57</v>
+      </c>
+      <c r="O6" s="10">
+        <v>23.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="42">
+        <v>28.57</v>
+      </c>
+      <c r="F7" s="42">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G7" s="42">
+        <v>33.590000000000003</v>
+      </c>
+      <c r="H7" s="42">
+        <v>1.55</v>
+      </c>
+      <c r="I7" s="42">
+        <v>-27.78</v>
+      </c>
+      <c r="K7" s="10">
+        <v>48.92</v>
+      </c>
+      <c r="L7" s="42">
+        <v>44.29</v>
+      </c>
+      <c r="M7" s="10">
+        <v>43.57</v>
+      </c>
+      <c r="N7" s="10">
+        <v>43.88</v>
+      </c>
+      <c r="O7" s="10">
+        <v>49.64</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G11" s="1"/>
+      <c r="M11" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1732,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A036AD0-7582-4D92-A231-DE51ED0E95AD}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E3" sqref="E3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1755,21 +2052,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="16"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1809,10 +2106,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1835,7 +2132,7 @@
         <v>18.75</v>
       </c>
       <c r="K3" s="35">
-        <v>19.07</v>
+        <v>11.4</v>
       </c>
       <c r="L3" s="37">
         <v>12.31</v>
@@ -1851,8 +2148,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="26" t="s">
         <v>16</v>
       </c>
@@ -1872,13 +2169,25 @@
       <c r="I4" s="35">
         <v>30.73</v>
       </c>
+      <c r="K4" s="42">
+        <v>36.6</v>
+      </c>
+      <c r="L4" s="42">
+        <v>41.03</v>
+      </c>
       <c r="M4" s="42">
         <v>32.47</v>
       </c>
+      <c r="N4" s="42">
+        <v>3.57</v>
+      </c>
+      <c r="O4" s="42">
+        <v>36.409999999999997</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="26" t="s">
         <v>48</v>
       </c>
@@ -1898,6 +2207,94 @@
       <c r="I5" s="35">
         <v>25.91</v>
       </c>
+      <c r="K5" s="42">
+        <v>38.46</v>
+      </c>
+      <c r="L5" s="42">
+        <v>46.39</v>
+      </c>
+      <c r="M5" s="42">
+        <v>31.79</v>
+      </c>
+      <c r="N5" s="42">
+        <v>3.61</v>
+      </c>
+      <c r="O5" s="42">
+        <v>32.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="42">
+        <v>45.36</v>
+      </c>
+      <c r="F6" s="52">
+        <v>19.13</v>
+      </c>
+      <c r="G6" s="42">
+        <v>38.86</v>
+      </c>
+      <c r="H6" s="52">
+        <v>22.51</v>
+      </c>
+      <c r="I6" s="52">
+        <v>38.86</v>
+      </c>
+      <c r="K6" s="42">
+        <v>4.62</v>
+      </c>
+      <c r="L6" s="42">
+        <v>7.22</v>
+      </c>
+      <c r="M6" s="42">
+        <v>1.55</v>
+      </c>
+      <c r="N6" s="42">
+        <v>4.12</v>
+      </c>
+      <c r="O6" s="42">
+        <v>22.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="52">
+        <v>58.06</v>
+      </c>
+      <c r="F7" s="52">
+        <v>38.46</v>
+      </c>
+      <c r="G7" s="52">
+        <v>53.72</v>
+      </c>
+      <c r="H7" s="52">
+        <v>33.51</v>
+      </c>
+      <c r="I7" s="52">
+        <v>16.95</v>
+      </c>
+      <c r="K7" s="42">
+        <v>31.12</v>
+      </c>
+      <c r="L7" s="42">
+        <v>31.28</v>
+      </c>
+      <c r="M7" s="42">
+        <v>28.21</v>
+      </c>
+      <c r="N7" s="42">
+        <v>26.67</v>
+      </c>
+      <c r="O7" s="42">
+        <v>29.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1914,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1D2C4E-0DC3-4E93-80C7-89BFF36994DD}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E3" sqref="E3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1937,21 +2334,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="16"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1991,10 +2388,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -2017,7 +2414,7 @@
         <v>-27.18</v>
       </c>
       <c r="K3" s="37">
-        <v>6.6</v>
+        <v>10.61</v>
       </c>
       <c r="L3" s="37">
         <v>-1.01</v>
@@ -2033,8 +2430,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -2054,13 +2451,25 @@
       <c r="I4" s="35">
         <v>-16.16</v>
       </c>
+      <c r="K4" s="42">
+        <v>18.09</v>
+      </c>
+      <c r="L4" s="42">
+        <v>19.100000000000001</v>
+      </c>
       <c r="M4" s="42">
         <v>21.21</v>
       </c>
+      <c r="N4" s="42">
+        <v>-1.01</v>
+      </c>
+      <c r="O4" s="42">
+        <v>12.12</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="26" t="s">
         <v>48</v>
       </c>
@@ -2079,9 +2488,94 @@
       <c r="I5" s="10">
         <v>-10.1</v>
       </c>
+      <c r="K5" s="42">
+        <v>24.24</v>
+      </c>
+      <c r="L5" s="42">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="M5" s="42">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="N5" s="42">
+        <v>4.55</v>
+      </c>
+      <c r="O5" s="42">
+        <v>7.58</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="38"/>
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10">
+        <v>11.58</v>
+      </c>
+      <c r="F6" s="10">
+        <v>10</v>
+      </c>
+      <c r="G6" s="10">
+        <v>5.88</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-4.26</v>
+      </c>
+      <c r="I6" s="10">
+        <v>5.88</v>
+      </c>
+      <c r="K6" s="42">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="L6" s="42">
+        <v>-2.5099999999999998</v>
+      </c>
+      <c r="M6" s="42">
+        <v>-0.5</v>
+      </c>
+      <c r="N6" s="42">
+        <v>-4.55</v>
+      </c>
+      <c r="O6" s="42">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="10">
+        <v>17.2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>6.38</v>
+      </c>
+      <c r="G7" s="10">
+        <v>14.29</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-1.59</v>
+      </c>
+      <c r="I7" s="10">
+        <v>-29.67</v>
+      </c>
+      <c r="K7" s="42">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="L7" s="42">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="M7" s="42">
+        <v>11.5</v>
+      </c>
+      <c r="N7" s="42">
+        <v>10.15</v>
+      </c>
+      <c r="O7" s="42">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2097,10 +2591,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CAF58B-48A0-4F9B-8783-9A2E0FD3237B}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2119,21 +2613,21 @@
       <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2172,10 +2666,10 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -2197,7 +2691,7 @@
         <v>41.33</v>
       </c>
       <c r="J3" s="37">
-        <v>35.35</v>
+        <v>37.19</v>
       </c>
       <c r="K3" s="37">
         <v>32.32</v>
@@ -2206,15 +2700,15 @@
         <v>31.31</v>
       </c>
       <c r="M3" s="42">
-        <v>27.78</v>
+        <v>32.32</v>
       </c>
       <c r="N3" s="37">
         <v>34.520000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -2233,13 +2727,25 @@
       <c r="H4" s="35">
         <v>65.31</v>
       </c>
+      <c r="J4" s="42">
+        <v>62.63</v>
+      </c>
+      <c r="K4" s="42">
+        <v>63.64</v>
+      </c>
       <c r="L4" s="42">
-        <v>34.67</v>
+        <v>70.64</v>
+      </c>
+      <c r="M4" s="42">
+        <v>35.68</v>
+      </c>
+      <c r="N4" s="42">
+        <v>51.26</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="26" t="s">
         <v>48</v>
       </c>
@@ -2258,6 +2764,94 @@
       <c r="H5" s="35">
         <v>63.45</v>
       </c>
+      <c r="J5" s="42">
+        <v>65.83</v>
+      </c>
+      <c r="K5" s="42">
+        <v>63.13</v>
+      </c>
+      <c r="L5" s="42">
+        <v>48.24</v>
+      </c>
+      <c r="M5" s="42">
+        <v>30.81</v>
+      </c>
+      <c r="N5" s="42">
+        <v>51.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="42">
+        <v>56.22</v>
+      </c>
+      <c r="E6" s="42">
+        <v>48.35</v>
+      </c>
+      <c r="F6" s="42">
+        <v>49.19</v>
+      </c>
+      <c r="G6" s="42">
+        <v>40.74</v>
+      </c>
+      <c r="H6" s="42">
+        <v>42.16</v>
+      </c>
+      <c r="J6" s="42">
+        <v>37.880000000000003</v>
+      </c>
+      <c r="K6" s="42">
+        <v>42.93</v>
+      </c>
+      <c r="L6" s="42">
+        <v>38.380000000000003</v>
+      </c>
+      <c r="M6" s="42">
+        <v>42.42</v>
+      </c>
+      <c r="N6" s="42">
+        <v>35.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="10">
+        <v>77.47</v>
+      </c>
+      <c r="E7" s="10">
+        <v>50</v>
+      </c>
+      <c r="F7" s="10">
+        <v>76.06</v>
+      </c>
+      <c r="G7" s="51">
+        <v>52.91</v>
+      </c>
+      <c r="H7" s="10">
+        <v>32.28</v>
+      </c>
+      <c r="J7" s="42">
+        <v>49.25</v>
+      </c>
+      <c r="K7" s="42">
+        <v>53.54</v>
+      </c>
+      <c r="L7" s="42">
+        <v>46.46</v>
+      </c>
+      <c r="M7" s="42">
+        <v>47.24</v>
+      </c>
+      <c r="N7" s="42">
+        <v>44.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2274,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2769504-2950-46E1-AD40-8B9DFC735BAD}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2297,21 +2891,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2320,21 +2914,21 @@
       <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" s="19" t="s">
@@ -2419,6 +3013,21 @@
       <c r="G5" s="35">
         <v>10.1</v>
       </c>
+      <c r="I5" s="27">
+        <v>58.8</v>
+      </c>
+      <c r="J5" s="27">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="K5" s="27">
+        <v>79</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="27">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
@@ -2436,6 +3045,11 @@
       <c r="G6" s="35">
         <v>10.1</v>
       </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
@@ -2450,10 +3064,14 @@
       <c r="E7" s="27">
         <v>89</v>
       </c>
-      <c r="F7" s="40"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="27">
         <v>10</v>
       </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -2468,11 +3086,16 @@
       <c r="E8" s="27">
         <v>89</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="27">
         <v>11.9</v>
       </c>
-      <c r="H8" s="41"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
@@ -2487,11 +3110,16 @@
       <c r="E9" s="27">
         <v>88</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="27">
         <v>11.3</v>
       </c>
-      <c r="H9" s="41"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="28" t="s">
@@ -2506,11 +3134,16 @@
       <c r="E10" s="27">
         <v>89</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="27">
         <v>10</v>
       </c>
-      <c r="H10" s="41"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
@@ -2519,7 +3152,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="40"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
     </row>
@@ -2528,7 +3161,7 @@
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="40"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
     </row>
@@ -2537,7 +3170,7 @@
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="40"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
     </row>
@@ -2573,7 +3206,7 @@
       <c r="E15" s="27">
         <v>88</v>
       </c>
-      <c r="F15" s="40"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="27">
         <v>10.3</v>
       </c>
@@ -2591,7 +3224,7 @@
       <c r="E16" s="27">
         <v>89</v>
       </c>
-      <c r="F16" s="40"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="27">
         <v>9.9</v>
       </c>
@@ -2609,15 +3242,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
@@ -2631,20 +3264,20 @@
       <c r="B26" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="I26" s="45" t="s">
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="I26" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C27" s="19" t="s">
@@ -2697,6 +3330,12 @@
       <c r="G28" s="10">
         <v>59.9</v>
       </c>
+      <c r="I28" s="10">
+        <v>46.79</v>
+      </c>
+      <c r="J28" s="10">
+        <v>34.53</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
@@ -2802,30 +3441,30 @@
       <c r="B34" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
@@ -2885,6 +3524,356 @@
       </c>
       <c r="G39" s="35">
         <v>79.290000000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="42">
+        <v>37.19</v>
+      </c>
+      <c r="D48" s="52">
+        <v>8.41</v>
+      </c>
+      <c r="E48" s="52">
+        <v>28.35</v>
+      </c>
+      <c r="F48" s="52">
+        <v>-1.08</v>
+      </c>
+      <c r="G48" s="52">
+        <v>37.25</v>
+      </c>
+    </row>
+    <row r="53" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C53" s="10">
+        <v>38.53</v>
+      </c>
+      <c r="D53" s="38">
+        <f>C53-$C$48</f>
+        <v>1.3400000000000034</v>
+      </c>
+      <c r="F53" s="10">
+        <v>28.99</v>
+      </c>
+      <c r="G53" s="38">
+        <f>F53-$E$48</f>
+        <v>0.63999999999999702</v>
+      </c>
+      <c r="I53" s="10">
+        <v>44.04</v>
+      </c>
+      <c r="J53" s="38">
+        <f>I53-$E$48</f>
+        <v>15.689999999999998</v>
+      </c>
+      <c r="L53" s="10">
+        <v>6.06</v>
+      </c>
+      <c r="M53" s="38">
+        <f>L53-$F$48</f>
+        <v>7.14</v>
+      </c>
+      <c r="O53" s="10">
+        <v>59.9</v>
+      </c>
+      <c r="P53" s="38">
+        <f>O53-$G$48</f>
+        <v>22.65</v>
+      </c>
+    </row>
+    <row r="54" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C54" s="10">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="D54" s="38">
+        <f t="shared" ref="D54:D61" si="0">C54-$C$48</f>
+        <v>39.659999999999997</v>
+      </c>
+      <c r="F54" s="10">
+        <v>34.53</v>
+      </c>
+      <c r="G54" s="38">
+        <f t="shared" ref="G54:G61" si="1">F54-$E$48</f>
+        <v>6.18</v>
+      </c>
+      <c r="I54" s="10">
+        <v>62.37</v>
+      </c>
+      <c r="J54" s="38">
+        <f t="shared" ref="J54:J61" si="2">I54-$E$48</f>
+        <v>34.019999999999996</v>
+      </c>
+      <c r="L54" s="10">
+        <v>26.63</v>
+      </c>
+      <c r="M54" s="38">
+        <f t="shared" ref="M54:M61" si="3">L54-$F$48</f>
+        <v>27.71</v>
+      </c>
+      <c r="O54" s="10">
+        <v>76.38</v>
+      </c>
+      <c r="P54" s="38">
+        <f t="shared" ref="P54:P61" si="4">O54-$G$48</f>
+        <v>39.129999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C55" s="10">
+        <v>82.57</v>
+      </c>
+      <c r="D55" s="38">
+        <f t="shared" si="0"/>
+        <v>45.379999999999995</v>
+      </c>
+      <c r="F55" s="10">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="G55" s="38">
+        <f t="shared" si="1"/>
+        <v>4.740000000000002</v>
+      </c>
+      <c r="I55" s="10">
+        <v>67.69</v>
+      </c>
+      <c r="J55" s="38">
+        <f t="shared" si="2"/>
+        <v>39.339999999999996</v>
+      </c>
+      <c r="L55" s="10">
+        <v>21.72</v>
+      </c>
+      <c r="M55" s="38">
+        <f t="shared" si="3"/>
+        <v>22.799999999999997</v>
+      </c>
+      <c r="O55" s="10">
+        <v>81.91</v>
+      </c>
+      <c r="P55" s="38">
+        <f t="shared" si="4"/>
+        <v>44.66</v>
+      </c>
+    </row>
+    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C56" s="10">
+        <v>56.88</v>
+      </c>
+      <c r="D56" s="38">
+        <f t="shared" si="0"/>
+        <v>19.690000000000005</v>
+      </c>
+      <c r="F56" s="10">
+        <v>34.06</v>
+      </c>
+      <c r="G56" s="38">
+        <f>F56-$E$48</f>
+        <v>5.7100000000000009</v>
+      </c>
+      <c r="I56" s="10">
+        <v>48.7</v>
+      </c>
+      <c r="J56" s="38">
+        <f t="shared" si="2"/>
+        <v>20.350000000000001</v>
+      </c>
+      <c r="L56" s="10">
+        <v>14.14</v>
+      </c>
+      <c r="M56" s="38">
+        <f t="shared" si="3"/>
+        <v>15.22</v>
+      </c>
+      <c r="O56" s="10">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="P56" s="38">
+        <f t="shared" si="4"/>
+        <v>30.930000000000007</v>
+      </c>
+    </row>
+    <row r="57" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C57" s="10">
+        <v>76.930000000000007</v>
+      </c>
+      <c r="D57" s="38">
+        <f t="shared" si="0"/>
+        <v>39.740000000000009</v>
+      </c>
+      <c r="F57" s="10">
+        <v>36.69</v>
+      </c>
+      <c r="G57" s="38">
+        <f t="shared" si="1"/>
+        <v>8.3399999999999963</v>
+      </c>
+      <c r="I57" s="10">
+        <v>58.76</v>
+      </c>
+      <c r="J57" s="38">
+        <f t="shared" si="2"/>
+        <v>30.409999999999997</v>
+      </c>
+      <c r="L57" s="10">
+        <v>25.25</v>
+      </c>
+      <c r="M57" s="38">
+        <f t="shared" si="3"/>
+        <v>26.33</v>
+      </c>
+      <c r="O57" s="10">
+        <v>77.39</v>
+      </c>
+      <c r="P57" s="38">
+        <f t="shared" si="4"/>
+        <v>40.14</v>
+      </c>
+    </row>
+    <row r="58" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C58" s="10">
+        <v>81.650000000000006</v>
+      </c>
+      <c r="D58" s="38">
+        <f t="shared" si="0"/>
+        <v>44.460000000000008</v>
+      </c>
+      <c r="F58" s="10">
+        <v>37.68</v>
+      </c>
+      <c r="G58" s="38">
+        <f t="shared" si="1"/>
+        <v>9.3299999999999983</v>
+      </c>
+      <c r="I58" s="10">
+        <v>62.56</v>
+      </c>
+      <c r="J58" s="38">
+        <f t="shared" si="2"/>
+        <v>34.21</v>
+      </c>
+      <c r="L58" s="10">
+        <v>27.92</v>
+      </c>
+      <c r="M58" s="38">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="O58" s="10">
+        <v>77.78</v>
+      </c>
+      <c r="P58" s="38">
+        <f t="shared" si="4"/>
+        <v>40.53</v>
+      </c>
+    </row>
+    <row r="59" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C59" s="10">
+        <v>33.03</v>
+      </c>
+      <c r="D59" s="38">
+        <f t="shared" si="0"/>
+        <v>-4.1599999999999966</v>
+      </c>
+      <c r="F59" s="10">
+        <v>25.36</v>
+      </c>
+      <c r="G59" s="38">
+        <f t="shared" si="1"/>
+        <v>-2.990000000000002</v>
+      </c>
+      <c r="I59" s="10">
+        <v>40.409999999999997</v>
+      </c>
+      <c r="J59" s="38">
+        <f t="shared" si="2"/>
+        <v>12.059999999999995</v>
+      </c>
+      <c r="L59" s="10">
+        <v>9.6</v>
+      </c>
+      <c r="M59" s="38">
+        <f t="shared" si="3"/>
+        <v>10.68</v>
+      </c>
+      <c r="O59" s="10">
+        <v>59.6</v>
+      </c>
+      <c r="P59" s="38">
+        <f t="shared" si="4"/>
+        <v>22.35</v>
+      </c>
+    </row>
+    <row r="60" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C60" s="10">
+        <v>69.72</v>
+      </c>
+      <c r="D60" s="38">
+        <f t="shared" si="0"/>
+        <v>32.53</v>
+      </c>
+      <c r="F60" s="10">
+        <v>43.48</v>
+      </c>
+      <c r="G60" s="38">
+        <f t="shared" si="1"/>
+        <v>15.129999999999995</v>
+      </c>
+      <c r="I60" s="10">
+        <v>61.34</v>
+      </c>
+      <c r="J60" s="38">
+        <f t="shared" si="2"/>
+        <v>32.99</v>
+      </c>
+      <c r="L60" s="10">
+        <v>24</v>
+      </c>
+      <c r="M60" s="38">
+        <f t="shared" si="3"/>
+        <v>25.08</v>
+      </c>
+      <c r="O60" s="10">
+        <v>79.8</v>
+      </c>
+      <c r="P60" s="38">
+        <f t="shared" si="4"/>
+        <v>42.55</v>
+      </c>
+    </row>
+    <row r="61" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C61" s="42">
+        <v>77.06</v>
+      </c>
+      <c r="D61" s="38">
+        <f t="shared" si="0"/>
+        <v>39.870000000000005</v>
+      </c>
+      <c r="F61" s="42">
+        <v>35.25</v>
+      </c>
+      <c r="G61" s="38">
+        <f t="shared" si="1"/>
+        <v>6.8999999999999986</v>
+      </c>
+      <c r="I61" s="42">
+        <v>65.459999999999994</v>
+      </c>
+      <c r="J61" s="38">
+        <f t="shared" si="2"/>
+        <v>37.109999999999992</v>
+      </c>
+      <c r="L61" s="42">
+        <v>24.75</v>
+      </c>
+      <c r="M61" s="38">
+        <f t="shared" si="3"/>
+        <v>25.83</v>
+      </c>
+      <c r="O61" s="42">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="P61" s="38">
+        <f t="shared" si="4"/>
+        <v>42.040000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -2899,4 +3888,182 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA62CC7-C021-4A05-AF0C-8FBF23A33ED5}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="42"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>